<commit_message>
Sai mssv của t
</commit_message>
<xml_diff>
--- a/process.xlsx
+++ b/process.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -41,6 +41,127 @@
   </si>
   <si>
     <t xml:space="preserve">KẾ HOẠCH THỰC HIỆN ĐỒ ÁN 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhận đề tài, tìm hiểu và xây dựng kế hoạch.
+</t>
+  </si>
+  <si>
+    <t>Thời gian</t>
+  </si>
+  <si>
+    <t>Phân tích đồ án, tìm hiểu thực tế</t>
+  </si>
+  <si>
+    <t>Thiết kế cơ sở dữ liệu vẽ mô hình ERD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tạo cơ sở dữ liệu trên SQL server </t>
+  </si>
+  <si>
+    <t>Đồng bộ cơ sở dữ liệu qua mạng Lan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thêm dữ liệu mẫu cơ sở dữ liệu </t>
+  </si>
+  <si>
+    <t>Bắt đầu tạo phần mềm:</t>
+  </si>
+  <si>
+    <t>Tạo form đăng nhập bao gồm thiết kế và code</t>
+  </si>
+  <si>
+    <t>Phân quyền truy cập cơ sở dữ liệu</t>
+  </si>
+  <si>
+    <t>Tạo form nhân viên, khách hàng, loại nhân viên</t>
+  </si>
+  <si>
+    <t>Tạo form kho, cửa hàng</t>
+  </si>
+  <si>
+    <t>Tạo form HSX, Loai SP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tạo form hóa đơn, chi tiết hóa đơn, sản phẩm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chức năng: </t>
+  </si>
+  <si>
+    <t>Tạo report hóa đơn, sản phẩm</t>
+  </si>
+  <si>
+    <t>Tạo biểu đồ doanh thu theo tháng, sản phẩm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giao hàng: xác định vị trí khách hàng và tìm đường( nếu được ) </t>
+  </si>
+  <si>
+    <t>11/9/2018 - 13/9/2018</t>
+  </si>
+  <si>
+    <t>14/9/2018- 15/9/2018</t>
+  </si>
+  <si>
+    <t>viết báo cáo, tạo powerpoint, tập luyện thuyết trình</t>
+  </si>
+  <si>
+    <t>Nộp sản phẩm</t>
+  </si>
+  <si>
+    <t>Kham khảo ý kiến của giáo viên</t>
+  </si>
+  <si>
+    <t>cùng thực hiện</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>08/10/2018-13/10/2018</t>
+  </si>
+  <si>
+    <t>15/10/2018-20/10/2018</t>
+  </si>
+  <si>
+    <t>22/10/2018-27/10/2018</t>
+  </si>
+  <si>
+    <t>Tính lương nhân viên</t>
+  </si>
+  <si>
+    <t>16/09/2018</t>
+  </si>
+  <si>
+    <t>17/09/2018</t>
+  </si>
+  <si>
+    <t>18/09/2018</t>
+  </si>
+  <si>
+    <t>19/09/2018</t>
+  </si>
+  <si>
+    <t>20/09/2018</t>
+  </si>
+  <si>
+    <t>22/09/2018</t>
+  </si>
+  <si>
+    <t>24/09/2018</t>
+  </si>
+  <si>
+    <t>25/09/2018</t>
+  </si>
+  <si>
+    <t>26/09/2018- 29/09/2018</t>
+  </si>
+  <si>
+    <t>04/10/2018 - 06/10/2018</t>
+  </si>
+  <si>
+    <t>Hoàn thiện,bổ sung, chỉnh sửa, kiểm tra lại phần mềm</t>
   </si>
   <si>
     <r>
@@ -59,137 +180,16 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve">
-Phan Thanh Nam - 16110163
+Phan Thanh Nam - 16110162
 Lâm Phước Bảo -  16110016</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Nhận đề tài, tìm hiểu và xây dựng kế hoạch.
-</t>
-  </si>
-  <si>
-    <t>Thời gian</t>
-  </si>
-  <si>
-    <t>Phân tích đồ án, tìm hiểu thực tế</t>
-  </si>
-  <si>
-    <t>Thiết kế cơ sở dữ liệu vẽ mô hình ERD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tạo cơ sở dữ liệu trên SQL server </t>
-  </si>
-  <si>
-    <t>Đồng bộ cơ sở dữ liệu qua mạng Lan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thêm dữ liệu mẫu cơ sở dữ liệu </t>
-  </si>
-  <si>
-    <t>Bắt đầu tạo phần mềm:</t>
-  </si>
-  <si>
-    <t>Tạo form đăng nhập bao gồm thiết kế và code</t>
-  </si>
-  <si>
-    <t>Phân quyền truy cập cơ sở dữ liệu</t>
-  </si>
-  <si>
-    <t>Tạo form nhân viên, khách hàng, loại nhân viên</t>
-  </si>
-  <si>
-    <t>Tạo form kho, cửa hàng</t>
-  </si>
-  <si>
-    <t>Tạo form HSX, Loai SP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tạo form hóa đơn, chi tiết hóa đơn, sản phẩm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chức năng: </t>
-  </si>
-  <si>
-    <t>Tạo report hóa đơn, sản phẩm</t>
-  </si>
-  <si>
-    <t>Tạo biểu đồ doanh thu theo tháng, sản phẩm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Giao hàng: xác định vị trí khách hàng và tìm đường( nếu được ) </t>
-  </si>
-  <si>
-    <t>11/9/2018 - 13/9/2018</t>
-  </si>
-  <si>
-    <t>14/9/2018- 15/9/2018</t>
-  </si>
-  <si>
-    <t>viết báo cáo, tạo powerpoint, tập luyện thuyết trình</t>
-  </si>
-  <si>
-    <t>Nộp sản phẩm</t>
-  </si>
-  <si>
-    <t>Kham khảo ý kiến của giáo viên</t>
-  </si>
-  <si>
-    <t>cùng thực hiện</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>08/10/2018-13/10/2018</t>
-  </si>
-  <si>
-    <t>15/10/2018-20/10/2018</t>
-  </si>
-  <si>
-    <t>22/10/2018-27/10/2018</t>
-  </si>
-  <si>
-    <t>Tính lương nhân viên</t>
-  </si>
-  <si>
-    <t>16/09/2018</t>
-  </si>
-  <si>
-    <t>17/09/2018</t>
-  </si>
-  <si>
-    <t>18/09/2018</t>
-  </si>
-  <si>
-    <t>19/09/2018</t>
-  </si>
-  <si>
-    <t>20/09/2018</t>
-  </si>
-  <si>
-    <t>22/09/2018</t>
-  </si>
-  <si>
-    <t>24/09/2018</t>
-  </si>
-  <si>
-    <t>25/09/2018</t>
-  </si>
-  <si>
-    <t>26/09/2018- 29/09/2018</t>
-  </si>
-  <si>
-    <t>04/10/2018 - 06/10/2018</t>
-  </si>
-  <si>
-    <t>Hoàn thiện,bổ sung, chỉnh sửa, kiểm tra lại phần mềm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,37 +507,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -570,15 +546,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -590,6 +557,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,7 +651,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -683,27 +683,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -735,24 +717,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -928,26 +892,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="73" style="1" customWidth="1"/>
@@ -958,411 +922,411 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" ht="27.75" customHeight="1">
+      <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:6" ht="50.25" thickBot="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:6" ht="28.5" customHeight="1" thickTop="1">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="23.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="33"/>
+    </row>
+    <row r="5" spans="1:6" ht="36.75" customHeight="1">
+      <c r="A5" s="34">
+        <v>1</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="34"/>
+      <c r="B6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="C6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="34"/>
+      <c r="B7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17.25" thickBot="1">
+      <c r="A8" s="34"/>
+      <c r="B8" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17.25" thickTop="1">
+      <c r="A9" s="35">
         <v>2</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
-        <v>1</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="27" t="s">
+      <c r="B9" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C9" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
-        <v>2</v>
-      </c>
-      <c r="B9" s="28" t="s">
+      <c r="D9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="36"/>
+      <c r="B10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C10" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="26" t="s">
+      <c r="D10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" ht="22.5" customHeight="1">
+      <c r="A11" s="36"/>
+      <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="36"/>
+      <c r="B12" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="20"/>
-    </row>
-    <row r="11" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="23"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="26" t="s">
+      <c r="D12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="36"/>
+      <c r="B13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="20"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>42</v>
+      <c r="C13" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="20"/>
-    </row>
-    <row r="14" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="33"/>
-      <c r="B14" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" ht="17.25" thickBot="1">
+      <c r="A14" s="37"/>
+      <c r="B14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" ht="17.25" thickTop="1">
+      <c r="A15" s="35">
+        <v>3</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C15" s="20" t="s">
         <v>43</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31">
-        <v>3</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>44</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="36"/>
+      <c r="B16" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" ht="17.25" thickBot="1">
+      <c r="A17" s="37"/>
+      <c r="B17" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C17" s="19" t="s">
         <v>45</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="20"/>
-    </row>
-    <row r="17" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33"/>
-      <c r="B17" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>46</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="21"/>
-    </row>
-    <row r="18" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31">
+        <v>32</v>
+      </c>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" ht="18" thickTop="1">
+      <c r="A18" s="35">
         <v>4</v>
       </c>
-      <c r="B18" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="28"/>
+      <c r="B18" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="20"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="29">
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="36"/>
+      <c r="B19" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="21">
         <v>43169</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="20"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="29">
+        <v>32</v>
+      </c>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="36"/>
+      <c r="B20" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="21">
         <v>43200</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="36"/>
+      <c r="B21" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="21">
+        <v>43141</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" ht="17.25" thickBot="1">
+      <c r="A22" s="37"/>
+      <c r="B22" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" ht="24" customHeight="1" thickTop="1">
+      <c r="A23" s="23">
+        <v>5</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="20"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="29">
-        <v>43141</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="20"/>
-    </row>
-    <row r="22" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="33"/>
-      <c r="B22" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="21"/>
-    </row>
-    <row r="23" spans="1:6" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34">
-        <v>5</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="28" t="s">
+      <c r="D23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="14"/>
+    </row>
+    <row r="24" spans="1:6" ht="24" customHeight="1">
+      <c r="A24" s="23">
+        <v>6</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="34">
-        <v>6</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="26" t="s">
+      <c r="D24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" ht="27" customHeight="1">
+      <c r="A25" s="23">
+        <v>7</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="20"/>
-    </row>
-    <row r="25" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34">
-        <v>7</v>
-      </c>
-      <c r="B25" s="26" t="s">
+      <c r="D25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:6" ht="24" customHeight="1" thickBot="1">
+      <c r="A26" s="24">
+        <v>8</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="20"/>
-    </row>
-    <row r="26" spans="1:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="35">
-        <v>8</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="27"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.25"/>
+        <v>32</v>
+      </c>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:6" ht="17.25" thickTop="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A22"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1370,24 +1334,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>